<commit_message>
linear programming files made for each guideline and each user, results exported to csv files
</commit_message>
<xml_diff>
--- a/TestingResults.xlsx
+++ b/TestingResults.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sotonac-my.sharepoint.com/personal/cb6g19_soton_ac_uk/Documents/Year 3/Semester 2/COMP3217/Labs/Lab2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:40009_{CE101C07-7A6B-4D4A-A5AC-7FF7F71658F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB23F11A-3E6E-43C6-9C61-17C788A8B357}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:40009_{CE101C07-7A6B-4D4A-A5AC-7FF7F71658F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5C1EFD6-C6D0-4593-9ED7-96099A70EF85}"/>
   <bookViews>
-    <workbookView xWindow="-35880" yWindow="7440" windowWidth="14400" windowHeight="7365" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestingResults" sheetId="1" r:id="rId1"/>
     <sheet name="AbnormalGuidelines" sheetId="4" r:id="rId2"/>
     <sheet name="ReportTable" sheetId="2" r:id="rId3"/>
-    <sheet name="GuideLine5" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">ReportTable!$A$1:$B$101</definedName>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
   <si>
     <t>Guideline</t>
   </si>
@@ -884,11 +883,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:Z101"/>
   <sheetViews>
-    <sheetView topLeftCell="O36" workbookViewId="0">
-      <selection sqref="A1:Z97"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -973,7 +971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1053,7 +1051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1133,7 +1131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1213,7 +1211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1453,7 +1451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1533,7 +1531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1693,7 +1691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1773,7 +1771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2013,7 +2011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2573,7 +2571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2733,7 +2731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2813,7 +2811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2893,7 +2891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3053,7 +3051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3213,7 +3211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3613,7 +3611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3773,7 +3771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3853,7 +3851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -4093,7 +4091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -4253,7 +4251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -4333,7 +4331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -4653,7 +4651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -4893,7 +4891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>50</v>
       </c>
@@ -5053,7 +5051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>52</v>
       </c>
@@ -5133,7 +5131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>53</v>
       </c>
@@ -5453,7 +5451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>57</v>
       </c>
@@ -5693,7 +5691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>60</v>
       </c>
@@ -5773,7 +5771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>61</v>
       </c>
@@ -6173,7 +6171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>66</v>
       </c>
@@ -6253,7 +6251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>67</v>
       </c>
@@ -6573,7 +6571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>71</v>
       </c>
@@ -6653,7 +6651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>72</v>
       </c>
@@ -6733,7 +6731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>73</v>
       </c>
@@ -6973,7 +6971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>76</v>
       </c>
@@ -7133,7 +7131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>78</v>
       </c>
@@ -7373,7 +7371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>81</v>
       </c>
@@ -7533,7 +7531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>83</v>
       </c>
@@ -8173,7 +8171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>91</v>
       </c>
@@ -8253,7 +8251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>92</v>
       </c>
@@ -8333,7 +8331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>93</v>
       </c>
@@ -8653,7 +8651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>97</v>
       </c>
@@ -8733,7 +8731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>98</v>
       </c>
@@ -8813,7 +8811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>99</v>
       </c>
@@ -8893,7 +8891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>100</v>
       </c>
@@ -8974,13 +8972,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Z101" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="25">
-      <filters>
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:Z101" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -8989,7 +8981,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6195ADA-A440-4234-9511-F7B94F678E06}">
   <dimension ref="A1:Z57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
@@ -13562,10 +13554,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E101"/>
+  <dimension ref="A1:B57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G56" sqref="G56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13574,1362 +13566,460 @@
     <col min="2" max="2" width="10.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>5</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>6</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>9</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>12</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>13</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>15</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>16</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>17</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>18</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>19</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>20</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>22</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <v>26</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>28</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="D16">
-        <v>30</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="D17">
-        <v>31</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="D18">
-        <v>32</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="D19">
-        <v>33</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="D20">
-        <v>35</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="D21">
-        <v>38</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>39</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="D23">
-        <v>41</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24">
-        <v>0</v>
-      </c>
-      <c r="D24">
-        <v>44</v>
-      </c>
-      <c r="E24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25">
-        <v>0</v>
-      </c>
-      <c r="D25">
-        <v>45</v>
-      </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26">
-        <v>0</v>
-      </c>
-      <c r="D26">
-        <v>46</v>
-      </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="D27">
-        <v>48</v>
-      </c>
-      <c r="E27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28">
-        <v>0</v>
-      </c>
-      <c r="D28">
-        <v>49</v>
-      </c>
-      <c r="E28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-      <c r="D29">
-        <v>51</v>
-      </c>
-      <c r="E29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30">
-        <v>0</v>
-      </c>
-      <c r="D30">
-        <v>54</v>
-      </c>
-      <c r="E30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="D31">
-        <v>55</v>
-      </c>
-      <c r="E31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="D32">
-        <v>56</v>
-      </c>
-      <c r="E32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33">
-        <v>32</v>
-      </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="D33">
-        <v>58</v>
-      </c>
-      <c r="E33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34">
-        <v>33</v>
-      </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-      <c r="D34">
-        <v>59</v>
-      </c>
-      <c r="E34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35">
-        <v>34</v>
-      </c>
-      <c r="B35">
-        <v>0</v>
-      </c>
-      <c r="D35">
-        <v>62</v>
-      </c>
-      <c r="E35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36">
-        <v>35</v>
-      </c>
-      <c r="B36">
-        <v>1</v>
-      </c>
-      <c r="D36">
-        <v>63</v>
-      </c>
-      <c r="E36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37">
-        <v>36</v>
-      </c>
-      <c r="B37">
-        <v>0</v>
-      </c>
-      <c r="D37">
-        <v>64</v>
-      </c>
-      <c r="E37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38">
-        <v>37</v>
-      </c>
-      <c r="B38">
-        <v>0</v>
-      </c>
-      <c r="D38">
-        <v>65</v>
-      </c>
-      <c r="E38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39">
-        <v>38</v>
-      </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-      <c r="D39">
-        <v>68</v>
-      </c>
-      <c r="E39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40">
-        <v>39</v>
-      </c>
-      <c r="B40">
-        <v>1</v>
-      </c>
-      <c r="D40">
-        <v>69</v>
-      </c>
-      <c r="E40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41">
-        <v>40</v>
-      </c>
-      <c r="B41">
-        <v>0</v>
-      </c>
-      <c r="D41">
-        <v>70</v>
-      </c>
-      <c r="E41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42">
-        <v>41</v>
-      </c>
-      <c r="B42">
-        <v>1</v>
-      </c>
-      <c r="D42">
-        <v>74</v>
-      </c>
-      <c r="E42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43">
-        <v>42</v>
-      </c>
-      <c r="B43">
-        <v>0</v>
-      </c>
-      <c r="D43">
-        <v>75</v>
-      </c>
-      <c r="E43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A44">
-        <v>43</v>
-      </c>
-      <c r="B44">
-        <v>0</v>
-      </c>
-      <c r="D44">
-        <v>77</v>
-      </c>
-      <c r="E44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45">
-        <v>44</v>
-      </c>
-      <c r="B45">
-        <v>1</v>
-      </c>
-      <c r="D45">
-        <v>79</v>
-      </c>
-      <c r="E45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46">
-        <v>45</v>
-      </c>
-      <c r="B46">
-        <v>1</v>
-      </c>
-      <c r="D46">
-        <v>80</v>
-      </c>
-      <c r="E46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47">
-        <v>46</v>
-      </c>
-      <c r="B47">
-        <v>1</v>
-      </c>
-      <c r="D47">
-        <v>82</v>
-      </c>
-      <c r="E47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48">
-        <v>47</v>
-      </c>
-      <c r="B48">
-        <v>0</v>
-      </c>
-      <c r="D48">
-        <v>84</v>
-      </c>
-      <c r="E48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A49">
-        <v>48</v>
-      </c>
-      <c r="B49">
-        <v>1</v>
-      </c>
-      <c r="D49">
-        <v>85</v>
-      </c>
-      <c r="E49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50">
-        <v>49</v>
-      </c>
-      <c r="B50">
-        <v>1</v>
-      </c>
-      <c r="D50">
-        <v>86</v>
-      </c>
-      <c r="E50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A51">
-        <v>50</v>
-      </c>
-      <c r="B51">
-        <v>0</v>
-      </c>
-      <c r="D51">
-        <v>87</v>
-      </c>
-      <c r="E51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A52">
-        <v>51</v>
-      </c>
-      <c r="B52">
-        <v>1</v>
-      </c>
-      <c r="D52">
-        <v>88</v>
-      </c>
-      <c r="E52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A53">
-        <v>52</v>
-      </c>
-      <c r="B53">
-        <v>0</v>
-      </c>
-      <c r="D53">
-        <v>89</v>
-      </c>
-      <c r="E53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54">
-        <v>53</v>
-      </c>
-      <c r="B54">
-        <v>0</v>
-      </c>
-      <c r="D54">
-        <v>90</v>
-      </c>
-      <c r="E54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A55">
-        <v>54</v>
-      </c>
-      <c r="B55">
-        <v>1</v>
-      </c>
-      <c r="D55">
-        <v>94</v>
-      </c>
-      <c r="E55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A56">
-        <v>55</v>
-      </c>
-      <c r="B56">
-        <v>1</v>
-      </c>
-      <c r="D56">
-        <v>95</v>
-      </c>
-      <c r="E56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A57">
-        <v>56</v>
-      </c>
-      <c r="B57">
-        <v>1</v>
-      </c>
-      <c r="D57">
-        <v>96</v>
-      </c>
-      <c r="E57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A58">
-        <v>57</v>
-      </c>
-      <c r="B58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A59">
-        <v>58</v>
-      </c>
-      <c r="B59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A60">
-        <v>59</v>
-      </c>
-      <c r="B60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A61">
-        <v>60</v>
-      </c>
-      <c r="B61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A62">
-        <v>61</v>
-      </c>
-      <c r="B62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A63">
-        <v>62</v>
-      </c>
-      <c r="B63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A64">
-        <v>63</v>
-      </c>
-      <c r="B64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A65">
-        <v>64</v>
-      </c>
-      <c r="B65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A66">
-        <v>65</v>
-      </c>
-      <c r="B66">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A67">
-        <v>66</v>
-      </c>
-      <c r="B67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A68">
-        <v>67</v>
-      </c>
-      <c r="B68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A69">
-        <v>68</v>
-      </c>
-      <c r="B69">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A70">
-        <v>69</v>
-      </c>
-      <c r="B70">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A71">
-        <v>70</v>
-      </c>
-      <c r="B71">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A72">
-        <v>71</v>
-      </c>
-      <c r="B72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A73">
-        <v>72</v>
-      </c>
-      <c r="B73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A74">
-        <v>73</v>
-      </c>
-      <c r="B74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A75">
-        <v>74</v>
-      </c>
-      <c r="B75">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A76">
-        <v>75</v>
-      </c>
-      <c r="B76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A77">
-        <v>76</v>
-      </c>
-      <c r="B77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A78">
-        <v>77</v>
-      </c>
-      <c r="B78">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A79">
-        <v>78</v>
-      </c>
-      <c r="B79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A80">
-        <v>79</v>
-      </c>
-      <c r="B80">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A81">
-        <v>80</v>
-      </c>
-      <c r="B81">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A82">
-        <v>81</v>
-      </c>
-      <c r="B82">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A83">
-        <v>82</v>
-      </c>
-      <c r="B83">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A84">
-        <v>83</v>
-      </c>
-      <c r="B84">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A85">
-        <v>84</v>
-      </c>
-      <c r="B85">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A86">
-        <v>85</v>
-      </c>
-      <c r="B86">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A87">
-        <v>86</v>
-      </c>
-      <c r="B87">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A88">
-        <v>87</v>
-      </c>
-      <c r="B88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A89">
-        <v>88</v>
-      </c>
-      <c r="B89">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A90">
-        <v>89</v>
-      </c>
-      <c r="B90">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A91">
-        <v>90</v>
-      </c>
-      <c r="B91">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A92">
-        <v>91</v>
-      </c>
-      <c r="B92">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A93">
-        <v>92</v>
-      </c>
-      <c r="B93">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A94">
-        <v>93</v>
-      </c>
-      <c r="B94">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A95">
-        <v>94</v>
-      </c>
-      <c r="B95">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A96">
-        <v>95</v>
-      </c>
-      <c r="B96">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A97">
-        <v>96</v>
-      </c>
-      <c r="B97">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A98">
-        <v>97</v>
-      </c>
-      <c r="B98">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A99">
-        <v>98</v>
-      </c>
-      <c r="B99">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A100">
-        <v>99</v>
-      </c>
-      <c r="B100">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A101">
-        <v>100</v>
-      </c>
-      <c r="B101">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:B101" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D2A65AE-CD5A-4734-BC79-8C729CE06EBE}">
-  <dimension ref="A1:B24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>4.6076621881661497</v>
-      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B2">
-        <v>3.6889711449494902</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B3">
-        <v>3.8046531799533398</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B4">
-        <v>2.8824344227974499</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B5">
-        <v>3.2473621599284099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B6">
-        <v>3.3936152393772199</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B7">
-        <v>3.72086091258205</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B8">
-        <v>3.6002734346157101</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B9">
-        <v>5.5363501122404104</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B10">
-        <v>4.6535119136964704</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B11">
-        <v>5.82005477994048</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B12">
-        <v>3.8692032981787401</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B13">
-        <v>6.3245188285027698</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="B14">
-        <v>4.7420371412062003</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="B15">
-        <v>5.4023819449062502</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="B16">
-        <v>5.7849292530996097</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="B17">
-        <v>6.3409684520441596</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="B18">
-        <v>6.6496031354351297</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="B19">
-        <v>6.7208083519146298</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="B20">
-        <v>5.3920205331100099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="B21">
-        <v>5.1302964796888597</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="B22">
-        <v>5.5328047302476397</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="B23">
-        <v>6.0289616823672603</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="B24">
-        <v>5.4964182774986803</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>45</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>46</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>48</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>49</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>51</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>54</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>55</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>56</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>58</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>59</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>62</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>63</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>64</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>65</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>68</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>69</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>70</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>74</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>75</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>77</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>79</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>80</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>82</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>84</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>85</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>86</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>87</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>88</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>89</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>90</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <v>94</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56">
+        <v>95</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <v>96</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>